<commit_message>
Missing variable rename, ggplots
</commit_message>
<xml_diff>
--- a/Data/VariableNames.xlsx
+++ b/Data/VariableNames.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephcaguioa/Desktop/SMUDS/MSDS6306_DDS/MSDS6306_CaseStudy2/Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7AD8F3-AEDE-9243-8E9C-191F6E9CA942}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="24" windowWidth="11460" windowHeight="7704"/>
+    <workbookView xWindow="11540" yWindow="1500" windowWidth="11460" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
   <si>
     <t>Age</t>
   </si>
@@ -196,15 +202,28 @@
   </si>
   <si>
     <t>YrsWtCurMgr</t>
+  </si>
+  <si>
+    <t>EducationField</t>
+  </si>
+  <si>
+    <t>EduField</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -237,26 +256,32 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -305,7 +330,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -338,9 +363,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -373,6 +415,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -548,20 +607,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" customWidth="1"/>
-    <col min="2" max="2" width="38.77734375" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="38.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -569,7 +628,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -577,7 +636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -585,7 +644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -593,7 +652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -601,7 +660,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -609,7 +668,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -617,7 +676,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -625,219 +684,227 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="17" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="18" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="23" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="26" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="29" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="31" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="32" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -847,24 +914,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Readability in VariableNames, age-income in Analysis
</commit_message>
<xml_diff>
--- a/Data/VariableNames.xlsx
+++ b/Data/VariableNames.xlsx
@@ -8,21 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephcaguioa/Desktop/SMUDS/MSDS6306_DDS/MSDS6306_CaseStudy2/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7AD8F3-AEDE-9243-8E9C-191F6E9CA942}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DE99B6-C740-5A4A-9598-BCC20CDA2145}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11540" yWindow="1500" windowWidth="11460" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4780" yWindow="1480" windowWidth="18220" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Names" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="93">
   <si>
     <t>Age</t>
   </si>
@@ -165,18 +163,9 @@
     <t>YrsCurrRole</t>
   </si>
   <si>
-    <t>JobInvolement</t>
-  </si>
-  <si>
     <t>WorkLifeBal</t>
   </si>
   <si>
-    <t>Modified Name</t>
-  </si>
-  <si>
-    <t>Original Name</t>
-  </si>
-  <si>
     <t>JobInvolvemt</t>
   </si>
   <si>
@@ -208,13 +197,115 @@
   </si>
   <si>
     <t>EduField</t>
+  </si>
+  <si>
+    <t>Original_Name</t>
+  </si>
+  <si>
+    <t>Modified_Name</t>
+  </si>
+  <si>
+    <t>Readable_Name</t>
+  </si>
+  <si>
+    <t>Business Travel</t>
+  </si>
+  <si>
+    <t>Daily Rate</t>
+  </si>
+  <si>
+    <t>Departent</t>
+  </si>
+  <si>
+    <t>Distance From Home</t>
+  </si>
+  <si>
+    <t>Education Field</t>
+  </si>
+  <si>
+    <t>Employee Count</t>
+  </si>
+  <si>
+    <t>Employee Number</t>
+  </si>
+  <si>
+    <t>Environment Satisfaction</t>
+  </si>
+  <si>
+    <t>Hourly Rate</t>
+  </si>
+  <si>
+    <t>Job Involvement</t>
+  </si>
+  <si>
+    <t>JobInvolvement</t>
+  </si>
+  <si>
+    <t>Job Level</t>
+  </si>
+  <si>
+    <t>Job Role</t>
+  </si>
+  <si>
+    <t>Job Satisfaction</t>
+  </si>
+  <si>
+    <t>Marital Status</t>
+  </si>
+  <si>
+    <t>Monthly Income</t>
+  </si>
+  <si>
+    <t>Monthly Rate</t>
+  </si>
+  <si>
+    <t>Number Companies Worked</t>
+  </si>
+  <si>
+    <t>Over 18</t>
+  </si>
+  <si>
+    <t>Percent Salary Hike</t>
+  </si>
+  <si>
+    <t>Performance Rating</t>
+  </si>
+  <si>
+    <t>Relationship Satisfaction</t>
+  </si>
+  <si>
+    <t>Standard Hours</t>
+  </si>
+  <si>
+    <t>Stock Option Level</t>
+  </si>
+  <si>
+    <t>Total Working Years</t>
+  </si>
+  <si>
+    <t>Training Times Last Year</t>
+  </si>
+  <si>
+    <t>Work Life Balance</t>
+  </si>
+  <si>
+    <t>Years At Company</t>
+  </si>
+  <si>
+    <t>Years In Current Role</t>
+  </si>
+  <si>
+    <t>Years Since Last Promotion</t>
+  </si>
+  <si>
+    <t>Years With Current Manager</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +321,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -256,19 +362,26 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,331 +721,416 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="2" max="2" width="38.83203125" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="1" t="s">
+    </row>
+    <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    </row>
+    <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    </row>
+    <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" t="s">
         <v>56</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>57</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>59</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>